<commit_message>
Update possible test units for each case
</commit_message>
<xml_diff>
--- a/Documents/TestCases.xlsx
+++ b/Documents/TestCases.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="User Online Reservation" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="53">
   <si>
     <t>Reservation Time is minimum of 2 Hours</t>
   </si>
@@ -50,9 +51,6 @@
     <t>User Reservation Scenario</t>
   </si>
   <si>
-    <t>Is Within Reservation Time</t>
-  </si>
-  <si>
     <t>Is Time 2 hours</t>
   </si>
   <si>
@@ -78,6 +76,114 @@
   </si>
   <si>
     <t>User is not allowed to reserve</t>
+  </si>
+  <si>
+    <t>From and To Less Than 2 hrs</t>
+  </si>
+  <si>
+    <t>From and To equals 2 hrs</t>
+  </si>
+  <si>
+    <t>From and To more than 2 hrs</t>
+  </si>
+  <si>
+    <t>From and To more than 2 hrs but %2 hrs</t>
+  </si>
+  <si>
+    <t>Is Within Reservation Time (9-21)</t>
+  </si>
+  <si>
+    <t>Is Within Reservation Time (9AM-9PM)</t>
+  </si>
+  <si>
+    <t>From time is less than 15 mins</t>
+  </si>
+  <si>
+    <t>From time is more than 15 mins</t>
+  </si>
+  <si>
+    <t>From time is 15 mins early</t>
+  </si>
+  <si>
+    <t>From time greater than current time (same day)</t>
+  </si>
+  <si>
+    <t>From time less than current time (same day)</t>
+  </si>
+  <si>
+    <t>From time equal current time (same day)</t>
+  </si>
+  <si>
+    <t>From time greater than current time (next day)</t>
+  </si>
+  <si>
+    <t>From time less than current time (next day)</t>
+  </si>
+  <si>
+    <t>From time equal current time (next day)</t>
+  </si>
+  <si>
+    <t>From time greater than current time (prev day)</t>
+  </si>
+  <si>
+    <t>From time less than current time (prev day)</t>
+  </si>
+  <si>
+    <t>From time equal current time (prev day)</t>
+  </si>
+  <si>
+    <t>To time greater than current time (same day)</t>
+  </si>
+  <si>
+    <t>To time less than current time (same day)</t>
+  </si>
+  <si>
+    <t>To time equal current time (same day)</t>
+  </si>
+  <si>
+    <t>To time greater than current time (next day)</t>
+  </si>
+  <si>
+    <t>To time less than current time (next day)</t>
+  </si>
+  <si>
+    <t>To time equal current time (next day)</t>
+  </si>
+  <si>
+    <t>To time greater than current time (prev day)</t>
+  </si>
+  <si>
+    <t>To time less than current time (prev day)</t>
+  </si>
+  <si>
+    <t>To time equal current time (prev day)</t>
+  </si>
+  <si>
+    <t>*** Reservation time is from schedule</t>
+  </si>
+  <si>
+    <t>From and To time is available (same day)</t>
+  </si>
+  <si>
+    <t>From and To time is NOT available (same day)</t>
+  </si>
+  <si>
+    <t>From NOT available and To time is available (same day)</t>
+  </si>
+  <si>
+    <t>From available and To time is NOT available (same day)</t>
+  </si>
+  <si>
+    <t>From and To time is available (next day)</t>
+  </si>
+  <si>
+    <t>From and To time is NOT available (next day)</t>
+  </si>
+  <si>
+    <t>From NOT available and To time is available (next day)</t>
+  </si>
+  <si>
+    <t>From available and To time is NOT available (next day)</t>
   </si>
 </sst>
 </file>
@@ -127,13 +233,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,18 +555,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="51" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -492,361 +598,544 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="E9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
         <v>12</v>
       </c>
-      <c r="D16" t="s">
-        <v>13</v>
-      </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
         <v>12</v>
       </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" t="s">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>